<commit_message>
melhorando codigo para possiveis erros
</commit_message>
<xml_diff>
--- a/hamburguerSP_top42.xlsx
+++ b/hamburguerSP_top42.xlsx
@@ -495,11 +495,11 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4.3</v>
+        <v>4.1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10 minutos</t>
+          <t>8 minutos</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11 minutos</t>
+          <t>10 minutos</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -573,11 +573,11 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>12 minutos</t>
+          <t>10 minutos</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -598,34 +598,34 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The Dog Haus</t>
+          <t>Cortés Asador</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R. Bandeira Paulista, 400 - Itaim Bibi, São Paulo - SP, 04532-000</t>
+          <t>144 Shopping Eldorado - Av. Rebouças, 3970 - Térreo - Loja - Pinheiros, São Paulo - SP, 05402-918</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>14 minutos</t>
+          <t>15 minutos</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>R$ 32 - R$ 35</t>
+          <t>R$ 45 - R$ 54</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>15 minutos</t>
+          <t>14 minutos</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -676,34 +676,34 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BLS</t>
+          <t>The Dog Haus</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>24</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R. Min. Jesuíno Cardoso, 149 - Itaim Bibi, São Paulo - SP, 04544-050</t>
+          <t>R. Bandeira Paulista, 400 - Itaim Bibi, São Paulo - SP, 04532-000</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>16 minutos</t>
+          <t>14 minutos</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>R$ 28 - R$ 43</t>
+          <t>R$ 32 - R$ 35</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -715,37 +715,41 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Donnies</t>
+          <t>Na Garagem</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>37</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R. João Cachoeira, 856 - Vila Nova Conceição</t>
+          <t>Rua Benjamim Egas, 301 Pinheiros, São Paulo, Brazil 05418-030</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>17 minutos</t>
+          <t>16 minutos</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>R$ 20 - R$ 23</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>R$ 27 - R$ 31</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>@nagaragem.hamburgueria</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
           <t>Não</t>
@@ -754,41 +758,37 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Na Garagem</t>
+          <t>Donnies</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>32</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rua Benjamim Egas, 301 Pinheiros, São Paulo, Brazil 05418-030</t>
+          <t>R. João Cachoeira, 856 - Vila Nova Conceição</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>6.5</v>
+        <v>6.2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>18 minutos</t>
+          <t>15 minutos</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>R$ 27 - R$ 31</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>@nagaragem.hamburgueria</t>
-        </is>
-      </c>
+          <t>R$ 20 - R$ 23</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>Não</t>
@@ -797,39 +797,39 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Caledonia Whisky &amp; Co.</t>
+          <t>Incêndio</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R. Vupabussu, 309 - Pinheiros, São Paulo - SP, 05429-040</t>
+          <t>Rua dos Pinheiros, 808, Pinheiros, Sao Paulo, Brazil 05422001</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>14 minutos</t>
+          <t>16 minutos</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>R$ 60 - R$ 60</t>
+          <t>R$ 45 - R$ 45</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>@caledoniabar</t>
+          <t>@incendiorestaurante</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -840,78 +840,78 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Patties</t>
+          <t>BLS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>31</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R. dos Pinheiros, 476 - Pinheiros, São Paulo - SP, 05422-001</t>
+          <t>R. Min. Jesuíno Cardoso, 149 - Itaim Bibi, São Paulo - SP, 04544-050</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>6.6</v>
+        <v>6.3</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>18 minutos</t>
+          <t>16 minutos</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>R$ 20 - R$ 22</t>
+          <t>R$ 28 - R$ 43</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pantchos</t>
+          <t>Z Deli Sandwiches</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R. Ramos Batista, 409 - Vila Olímpia</t>
+          <t>R. Leopoldo Couto Magalhães Júnior, 785 - Itaim Bibi, São Paulo - SP, 04542-011</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>16 minutos</t>
+          <t>17 minutos</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>R$ 22 - R$ 37</t>
+          <t>R$ 44 - R$ 48</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>@pantchoshouse</t>
+          <t>@zdelisandwiches</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -922,39 +922,39 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Z Deli Sandwiches</t>
+          <t>Caledonia Whisky &amp; Co.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R. Leopoldo Couto Magalhães Júnior, 785 - Itaim Bibi, São Paulo - SP, 04542-011</t>
+          <t>R. Vupabussu, 309 - Pinheiros, São Paulo - SP, 05429-040</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>19 minutos</t>
+          <t>14 minutos</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>R$ 44 - R$ 48</t>
+          <t>R$ 60 - R$ 60</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>@zdelisandwiches</t>
+          <t>@caledoniabar</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -983,11 +983,11 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>18 minutos</t>
+          <t>16 minutos</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1004,37 +1004,41 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>All In Burger</t>
+          <t>Matilda Lanches</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>36</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R. Dr. Renato Paes de Barros, 465 - Itaim Bibi, São Paulo - SP, 04530-000</t>
+          <t>R. Mateus Grou, 31 - Pinheiros, São Paulo - SP, 05415-050</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>15 minutos</t>
+          <t>17 minutos</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>R$ 32 - R$ 42</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
+          <t>R$ 29 - R$ 41</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>@matildalanches</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1043,25 +1047,25 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Incêndio</t>
+          <t>Patties</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Rua dos Pinheiros, 808, Pinheiros, Sao Paulo, Brazil 05422001</t>
+          <t>R. dos Pinheiros, 476 - Pinheiros, São Paulo - SP, 05422-001</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1070,41 +1074,37 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>R$ 45 - R$ 45</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>@incendiorestaurante</t>
-        </is>
-      </c>
+          <t>R$ 20 - R$ 22</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ritz</t>
+          <t>Pantchos</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Brig. Faria Lima, 2232 - Jd. Paulistano</t>
+          <t>R. Ramos Batista, 409 - Vila Olímpia</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>6.9</v>
+        <v>6.6</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1113,53 +1113,53 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>R$ 67 - R$ 77</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
+          <t>R$ 22 - R$ 37</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>@pantchoshouse</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Debetti</t>
+          <t>Ritz</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Av.Brig. Luiz Antonio, 3935 - Jardins</t>
+          <t>Brig. Faria Lima, 2232 - Jd. Paulistano</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>6.9</v>
+        <v>6.7</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>15 minutos</t>
+          <t>14 minutos</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>R$ 30 - R$ 46</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>@debetti</t>
-        </is>
-      </c>
+          <t>R$ 67 - R$ 77</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
           <t>Sim</t>
@@ -1168,34 +1168,34 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cortés Asador</t>
+          <t>All In Burger</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>39</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>144 Shopping Eldorado - Av. Rebouças, 3970 - Térreo - Loja - Pinheiros, São Paulo - SP, 05402-918</t>
+          <t>R. Dr. Renato Paes de Barros, 465 - Itaim Bibi, São Paulo - SP, 04530-000</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>16 minutos</t>
+          <t>15 minutos</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>R$ 45 - R$ 54</t>
+          <t>R$ 32 - R$ 42</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1207,39 +1207,39 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Matilda Lanches</t>
+          <t>Buzina</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>R. Mateus Grou, 31 - Pinheiros, São Paulo - SP, 05415-050</t>
+          <t>R. Padre Carvalho, 30 - Pinheiros, São Paulo - SP, 05429-040</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>7.1</v>
+        <v>6.9</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>20 minutos</t>
+          <t>15 minutos</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>R$ 29 - R$ 41</t>
+          <t>R$ 33 - R$ 38</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>@matildalanches</t>
+          <t>@buzinaburgers</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1250,37 +1250,41 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lanchonete da Cidade</t>
+          <t>Z Deli Sandwiches</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>R. Coropés, 51 - Pinheiros - SP</t>
+          <t>R. Francisco Leitão, 16 - Pinheiros, São Paulo - SP, 05414-020</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>16 minutos</t>
+          <t>19 minutos</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>R$ 39 - R$ 43</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
+          <t>R$ 44 - R$ 48</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>@zdelisandwiches</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
           <t>Sim</t>
@@ -1307,11 +1311,11 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7.3</v>
+        <v>7.1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>19 minutos</t>
+          <t>17 minutos</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1332,44 +1336,40 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Buzina</t>
+          <t>Lanchonete da Cidade</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>R. Padre Carvalho, 30 - Pinheiros, São Paulo - SP, 05429-040</t>
+          <t>R. Coropés, 51 - Pinheiros - SP</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>7.4</v>
+        <v>7.2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>17 minutos</t>
+          <t>16 minutos</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>R$ 33 - R$ 38</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>@buzinaburgers</t>
-        </is>
-      </c>
+          <t>R$ 39 - R$ 43</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -1393,11 +1393,11 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>19 minutos</t>
+          <t>17 minutos</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1414,41 +1414,37 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Z Deli Sandwiches</t>
+          <t>La Borratxeria</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>R. Francisco Leitão, 16 - Pinheiros, São Paulo - SP, 05414-020</t>
+          <t>R. João Moura, 541 - Pinheiros, São Paulo - SP, 05412-001</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>7.5</v>
+        <v>7.9</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>21 minutos</t>
+          <t>20 minutos</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>R$ 44 - R$ 48</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>@zdelisandwiches</t>
-        </is>
-      </c>
+          <t>R$ 40 - R$ 46</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
           <t>Sim</t>
@@ -1500,25 +1496,25 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Raw Burger</t>
+          <t>Coringa do Beco</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>38</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>R. Aspicuelta, 176 - Vila Madalena, São Paulo - SP, 05433-010</t>
+          <t>Rua Harmonia, 68a - Sumarezinho, São Paulo - SP, 05435-000</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1527,14 +1523,10 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>R$ 47 - R$ 57</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>@raw.burger</t>
-        </is>
-      </c>
+          <t>R$ 35 - R$ 36</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1543,39 +1535,39 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Z Deli Sandwiches</t>
+          <t>Debetti</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>R. Oscar Freire, 164 - Jardim Paulista, São Paulo - SP, 01426-000</t>
+          <t>Av. Brigadeiro Luís Antônio, 3935 - Jardim Paulista, São Paulo - SP, 01401-001</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>8.6</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>21 minutos</t>
+          <t>19 minutos</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>R$ 44 - R$ 48</t>
+          <t>R$ 30 - R$ 46</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>@zdelisandwiches</t>
+          <t>@debetti</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1586,37 +1578,41 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Coringa do Beco</t>
+          <t>Raw Burger</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>15</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Rua Harmonia, 68a - Sumarezinho, São Paulo - SP, 05435-000</t>
+          <t>R. Aspicuelta, 176 - Vila Madalena, São Paulo - SP, 05433-010</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>8.699999999999999</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>22 minutos</t>
+          <t>20 minutos</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>R$ 35 - R$ 36</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
+          <t>R$ 47 - R$ 57</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>@raw.burger</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1643,11 +1639,11 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>8.9</v>
+        <v>8.4</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>20 minutos</t>
+          <t>18 minutos</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1664,150 +1660,150 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Big Kahuna</t>
+          <t>Z Deli Sandwiches</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Alameda Lorena, 53 - Jardim Paulista, São Paulo - SP, 01424-001</t>
+          <t>R. Oscar Freire, 164 - Jardim Paulista, São Paulo - SP, 01426-000</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>22 minutos</t>
+          <t>19 minutos</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>R$ 30 - R$ 40</t>
+          <t>R$ 44 - R$ 48</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>@bigkahunaburgerr</t>
+          <t>@zdelisandwiches</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ritz</t>
+          <t>Z Deli Restaurante</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Al. Franca, 1088 - Jardim Paulista</t>
+          <t>Alameda Lorena, 1689 - Jardim Paulista, São Paulo - SP, 01424-007</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>23 minutos</t>
+          <t>21 minutos</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>R$ 67 - R$ 77</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr"/>
+          <t>R$ 67 - R$ 67</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>@zdelisandwiches</t>
+        </is>
+      </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Z Deli Restaurante</t>
+          <t>Ritz</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Alameda Lorena, 1689 - Jardim Paulista, São Paulo - SP, 01424-007</t>
+          <t>Al. Franca, 1088 - Jardim Paulista</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>23 minutos</t>
+          <t>21 minutos</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>R$ 67 - R$ 67</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>@zdelisandwiches</t>
-        </is>
-      </c>
+          <t>R$ 67 - R$ 77</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>La Borratxeria</t>
+          <t>Big Kahuna</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>29</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>R. João Moura, 541 - Pinheiros, São Paulo - SP, 05412-001</t>
+          <t>Alameda Lorena, 53 - Jardim Paulista, São Paulo - SP, 01424-001</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1816,51 +1812,55 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>R$ 40 - R$ 46</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
+          <t>R$ 30 - R$ 40</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>@bigkahunaburgerr</t>
+        </is>
+      </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Coa Bar y Parrilla</t>
+          <t>Jota Hamburgers</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>42</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Alameda dos Anapurus, 1631 - Indianópolis, São Paulo - SP, 04087-006</t>
+          <t>R. Pamplona, 529 - Jardim Paulista, São Paulo - SP, 01405-100</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>9.699999999999999</v>
+        <v>9.6</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>21 minutos</t>
+          <t>26 minutos</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>R$ 49 - R$ 49</t>
+          <t>R$ 16 - R$ 18</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>@coa.bar</t>
+          <t>@jotahamburgers</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -1871,39 +1871,39 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Jota Hamburgers</t>
+          <t>Coa Bar y Parrilla</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>R. Pamplona, 529 - Jardim Paulista, São Paulo - SP, 01405-100</t>
+          <t>Alameda dos Anapurus, 1631 - Indianópolis, São Paulo - SP, 04087-006</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>9.800000000000001</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>28 minutos</t>
+          <t>21 minutos</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>R$ 16 - R$ 18</t>
+          <t>R$ 49 - R$ 49</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>@jotahamburgers</t>
+          <t>@coa.bar</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -1971,11 +1971,11 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>10.6</v>
+        <v>10.2</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>25 minutos</t>
+          <t>23 minutos</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1992,37 +1992,41 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Castro Burger</t>
+          <t>Frank &amp; Charles</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>R. Joaquim Távora, 1517 - Vila Mariana, São Paulo - SP, 04015-003</t>
+          <t>Rua Tinhorão, 130 - Higienópolis, São Paulo - SP, 01241-030</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>10.7</v>
+        <v>10.3</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>28 minutos</t>
+          <t>25 minutos</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>R$ 34 - R$ 36</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr"/>
+          <t>R$ 41 - R$ 47</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>@frankcharles1885</t>
+        </is>
+      </c>
       <c r="I39" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2031,41 +2035,37 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Frank &amp; Charles</t>
+          <t>Castro Burger</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>40</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Rua Tinhorão, 130 - Higienópolis, São Paulo - SP, 01241-030</t>
+          <t>R. Joaquim Távora, 1517 - Vila Mariana, São Paulo - SP, 04015-003</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>10.8</v>
+        <v>10.5</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>27 minutos</t>
+          <t>26 minutos</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>R$ 41 - R$ 47</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>@frankcharles1885</t>
-        </is>
-      </c>
+          <t>R$ 34 - R$ 36</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2074,25 +2074,25 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ici Bistrô</t>
+          <t>Holy Burger</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Rua Mato Grosso, 396, São Paulo, Brazil 01243-020</t>
+          <t>R. Dr. Cesário Mota Júnior, 527 - Vila Buarque, São Paulo - SP, 01221-020</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>11.1</v>
+        <v>11</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>@ici_bistro</t>
+          <t>@holyburgersp</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2117,111 +2117,107 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Elevado Conselheiro</t>
+          <t>Lanchonete da Cidade</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>R. Conselheiro Ramalho, 800 - Bela Vista, São Paulo - SP, 01325-000</t>
+          <t>Av. Higienópolis, 618 Piso Veiga Filho - Higienópolis - SP</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>11.2</v>
+        <v>11</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>32 minutos</t>
+          <t>27 minutos</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>R$ 86 - R$ 86</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>@elevado_conselheiro</t>
-        </is>
-      </c>
+          <t>R$ 39 - R$ 43</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Z Deli Sandwiches</t>
+          <t>Elevado Conselheiro</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>R. Bento Freitas, 314 - Vila Buarque, São Paulo - SP, 01220-000</t>
+          <t>R. Conselheiro Ramalho, 800 - Bela Vista, São Paulo - SP, 01325-000</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>11.3</v>
+        <v>11</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>31 minutos</t>
+          <t>30 minutos</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>R$ 44 - R$ 48</t>
+          <t>R$ 86 - R$ 86</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>@zdelisandwiches</t>
+          <t>@elevado_conselheiro</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Lanchonete da Cidade</t>
+          <t>Ici Bistrô</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Av. Higienópolis, 618 Piso Veiga Filho - Higienópolis - SP</t>
+          <t>Rua Mato Grosso, 396, São Paulo, Brazil 01243-020</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>11.4</v>
+        <v>11.1</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2230,37 +2226,41 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>R$ 39 - R$ 43</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr"/>
+          <t>R$ 59 - R$ 59</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>@ici_bistro</t>
+        </is>
+      </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Holy Burger</t>
+          <t>Z Deli Sandwiches</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>R. Dr. Cesário Mota Júnior, 527 - Vila Buarque, São Paulo - SP, 01221-020</t>
+          <t>R. Bento Freitas, 314 - Vila Buarque, São Paulo - SP, 01220-000</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>11.5</v>
+        <v>11.3</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2269,50 +2269,50 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>R$ 59 - R$ 59</t>
+          <t>R$ 44 - R$ 48</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>@holyburgersp</t>
+          <t>@zdelisandwiches</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ecully Charbon</t>
+          <t>Xepa</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>R. Min. Ferreira Alves, 825 - Pompeia, São Paulo - SP, 05009-060</t>
+          <t>R. Jaguaribe, 529 - Consolação, São Paulo - SP, 01224-001</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>11.7</v>
+        <v>11.3</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>28 minutos</t>
+          <t>30 minutos</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>R$ 42 - R$ 42</t>
+          <t>R$ 50 - R$ 59</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -2324,37 +2324,41 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Xepa</t>
+          <t>Chimichurri Parrilla</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>R. Jaguaribe, 529 - Consolação, São Paulo - SP, 01224-001</t>
+          <t>Av. Prof. Alfonso Bovero, 730 - Perdizes, São Paulo - SP, 05019-010</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>11.8</v>
+        <v>11.4</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>32 minutos</t>
+          <t>27 minutos</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>R$ 50 - R$ 59</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr"/>
+          <t>R$ 42 - R$ 48</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>@chimi_parrilla</t>
+        </is>
+      </c>
       <c r="I47" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2363,41 +2367,37 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Chimichurri Parrilla</t>
+          <t>Ecully Charbon</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Av. Prof. Alfonso Bovero, 730 - Perdizes, São Paulo - SP, 05019-010</t>
+          <t>R. Min. Ferreira Alves, 825 - Pompeia, São Paulo - SP, 05009-060</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>11.9</v>
+        <v>11.7</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>29 minutos</t>
+          <t>28 minutos</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>R$ 42 - R$ 48</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>@chimi_parrilla</t>
-        </is>
-      </c>
+          <t>R$ 42 - R$ 42</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2406,25 +2406,25 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>The Bear Burger</t>
+          <t>Seven Kings</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>34</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>R. Caiubí, 1537 - Perdizes, São Paulo - SP, 05010-000</t>
+          <t>R. Dr. Cândido Espinheira, 812 - Perdizes, São Paulo - SP, 05004-000</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>12.3</v>
+        <v>11.9</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2433,92 +2433,92 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>R$ 41 - R$ 42</t>
+          <t>R$ 25 - R$ 44</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Seven Kings</t>
+          <t>The Pitchers</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>R. Dr. Cândido Espinheira, 812 - Perdizes, São Paulo - SP, 05004-000</t>
+          <t>R. Dr. Bacelar, 1155 - Vila Clementino, São Paulo - SP, 04026-002</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>12.4</v>
+        <v>12</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>32 minutos</t>
+          <t>23 minutos</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>R$ 25 - R$ 44</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
+          <t>R$ 35 - R$ 38</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>@thepitchers_burger_baseball</t>
+        </is>
+      </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>The Pitchers</t>
+          <t>The Bear Burger</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>R. Dr. Bacelar, 1155 - Vila Clementino, São Paulo - SP, 04026-002</t>
+          <t>R. Caiubí, 1537 - Perdizes, São Paulo - SP, 05010-000</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>13.3</v>
+        <v>12.3</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>25 minutos</t>
+          <t>30 minutos</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>R$ 35 - R$ 38</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>@thepitchers_burger_baseball</t>
-        </is>
-      </c>
+          <t>R$ 41 - R$ 42</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2588,11 +2588,11 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>14.8</v>
+        <v>14.6</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>35 minutos</t>
+          <t>33 minutos</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2627,11 +2627,11 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>18.9</v>
+        <v>18.7</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>43 minutos</t>
+          <t>41 minutos</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2666,7 +2666,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>18.9</v>
+        <v>18.8</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -2709,11 +2709,11 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>19.3</v>
+        <v>19</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>44 minutos</t>
+          <t>42 minutos</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2795,11 +2795,11 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>20.1</v>
+        <v>19.9</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>47 minutos</t>
+          <t>45 minutos</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">

</xml_diff>